<commit_message>
added support for spouse from within the family
</commit_message>
<xml_diff>
--- a/bushnaq.xlsx
+++ b/bushnaq.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="128">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -335,9 +335,6 @@
   </si>
   <si>
     <t xml:space="preserve">Dima</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (geschieden), should be a reference</t>
   </si>
   <si>
     <t xml:space="preserve">Tareq</t>
@@ -637,13 +634,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E99" activeCellId="0" sqref="E99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G83" activeCellId="0" sqref="G83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -2435,16 +2432,21 @@
       <c r="B83" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C83" s="5" t="s">
-        <v>42</v>
+      <c r="C83" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>40</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
-      <c r="I83" s="6" t="s">
-        <v>105</v>
+      <c r="G83" s="5" t="str">
+        <f aca="false">$C$26</f>
+        <v>Bassil</v>
+      </c>
+      <c r="H83" s="0" t="str">
+        <f aca="false">$C$82</f>
+        <v>Dima</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2452,11 +2454,11 @@
         <f aca="false">ROW()</f>
         <v>84</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>9</v>
+      <c r="B84" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>40</v>
@@ -2464,7 +2466,7 @@
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="5" t="str">
-        <f aca="false">$C$83</f>
+        <f aca="false">$C$26</f>
         <v>Bassil</v>
       </c>
       <c r="H84" s="0" t="str">
@@ -2481,20 +2483,20 @@
         <v>12</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>40</v>
+        <v>106</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
-      <c r="G85" s="5" t="str">
-        <f aca="false">$C$83</f>
-        <v>Bassil</v>
+      <c r="G85" s="0" t="str">
+        <f aca="false">$C$80</f>
+        <v>Walid</v>
       </c>
       <c r="H85" s="0" t="str">
-        <f aca="false">$C$82</f>
-        <v>Dima</v>
+        <f aca="false">$C$81</f>
+        <v>Fadwa</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,25 +2504,17 @@
         <f aca="false">ROW()</f>
         <v>86</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C86" s="0" t="s">
+      <c r="B86" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D86" s="0" t="s">
-        <v>11</v>
+      <c r="D86" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
-      <c r="G86" s="0" t="str">
-        <f aca="false">$C$80</f>
-        <v>Walid</v>
-      </c>
-      <c r="H86" s="0" t="str">
-        <f aca="false">$C$81</f>
-        <v>Fadwa</v>
-      </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
@@ -2530,37 +2524,45 @@
       <c r="B87" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C87" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D87" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
+      <c r="G87" s="5" t="str">
+        <f aca="false">$C$86</f>
+        <v>Motaz</v>
+      </c>
+      <c r="H87" s="0" t="str">
+        <f aca="false">$C$85</f>
+        <v>Rania</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
         <f aca="false">ROW()</f>
         <v>88</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>9</v>
+      <c r="B88" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>110</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
       <c r="G88" s="5" t="str">
-        <f aca="false">$C$87</f>
+        <f aca="false">$C$86</f>
         <v>Motaz</v>
       </c>
       <c r="H88" s="0" t="str">
-        <f aca="false">$C$86</f>
+        <f aca="false">$C$85</f>
         <v>Rania</v>
       </c>
     </row>
@@ -2575,18 +2577,18 @@
       <c r="C89" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="D89" s="5" t="s">
-        <v>109</v>
+      <c r="D89" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
-      <c r="G89" s="5" t="str">
-        <f aca="false">$C$87</f>
-        <v>Motaz</v>
+      <c r="G89" s="0" t="str">
+        <f aca="false">$C$80</f>
+        <v>Walid</v>
       </c>
       <c r="H89" s="0" t="str">
-        <f aca="false">$C$86</f>
-        <v>Rania</v>
+        <f aca="false">$C$81</f>
+        <v>Fadwa</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,65 +2596,65 @@
         <f aca="false">ROW()</f>
         <v>90</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C90" s="0" t="s">
+      <c r="B90" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="D90" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
-      <c r="G90" s="0" t="str">
-        <f aca="false">$C$80</f>
-        <v>Walid</v>
-      </c>
-      <c r="H90" s="0" t="str">
-        <f aca="false">$C$81</f>
-        <v>Fadwa</v>
-      </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <f aca="false">ROW()</f>
         <v>91</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>41</v>
+      <c r="B91" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>113</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
+      <c r="G91" s="5" t="str">
+        <f aca="false">$C$90</f>
+        <v>Samer</v>
+      </c>
+      <c r="H91" s="0" t="str">
+        <f aca="false">$C$89</f>
+        <v>Manal</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
         <f aca="false">ROW()</f>
         <v>92</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>12</v>
+      <c r="B92" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>114</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
       <c r="G92" s="5" t="str">
-        <f aca="false">$C$91</f>
+        <f aca="false">$C$90</f>
         <v>Samer</v>
       </c>
       <c r="H92" s="0" t="str">
-        <f aca="false">$C$90</f>
+        <f aca="false">$C$89</f>
         <v>Manal</v>
       </c>
     </row>
@@ -2661,23 +2663,23 @@
         <f aca="false">ROW()</f>
         <v>93</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C93" s="0" t="s">
+      <c r="B93" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C93" s="5" t="s">
         <v>115</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="5" t="str">
-        <f aca="false">$C$91</f>
+        <f aca="false">$C$90</f>
         <v>Samer</v>
       </c>
       <c r="H93" s="0" t="str">
-        <f aca="false">$C$90</f>
+        <f aca="false">$C$89</f>
         <v>Manal</v>
       </c>
     </row>
@@ -2689,21 +2691,20 @@
       <c r="B94" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="C94" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="D94" s="5" t="s">
-        <v>113</v>
+      <c r="D94" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="E94" s="4"/>
-      <c r="F94" s="4"/>
-      <c r="G94" s="5" t="str">
-        <f aca="false">$C$91</f>
-        <v>Samer</v>
+      <c r="G94" s="0" t="str">
+        <f aca="false">$C$80</f>
+        <v>Walid</v>
       </c>
       <c r="H94" s="0" t="str">
-        <f aca="false">$C$90</f>
-        <v>Manal</v>
+        <f aca="false">$C$81</f>
+        <v>Fadwa</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2711,86 +2712,88 @@
         <f aca="false">ROW()</f>
         <v>95</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C95" s="0" t="s">
+      <c r="B95" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D95" s="0" t="s">
-        <v>11</v>
+      <c r="D95" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="E95" s="4"/>
-      <c r="G95" s="0" t="str">
+    </row>
+    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>96</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E96" s="4"/>
+      <c r="G96" s="0" t="str">
+        <f aca="false">$C$95</f>
+        <v>Eddie</v>
+      </c>
+      <c r="H96" s="0" t="str">
+        <f aca="false">$C$94</f>
+        <v>Mona</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>97</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G97" s="0" t="str">
         <f aca="false">$C$80</f>
         <v>Walid</v>
       </c>
-      <c r="H95" s="0" t="str">
+      <c r="H97" s="0" t="str">
         <f aca="false">$C$81</f>
         <v>Fadwa</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="n">
-        <f aca="false">ROW()</f>
-        <v>96</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E96" s="4"/>
-    </row>
-    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="n">
-        <f aca="false">ROW()</f>
-        <v>97</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C97" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E97" s="4"/>
-      <c r="G97" s="0" t="str">
-        <f aca="false">$C$96</f>
-        <v>Eddie</v>
-      </c>
-      <c r="H97" s="0" t="str">
-        <f aca="false">$C$95</f>
-        <v>Mona</v>
-      </c>
-    </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
         <f aca="false">ROW()</f>
         <v>98</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>9</v>
+      <c r="B98" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="D98" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="E98" s="4" t="n">
+        <v>18537</v>
+      </c>
       <c r="G98" s="0" t="str">
-        <f aca="false">$C$80</f>
-        <v>Walid</v>
+        <f aca="false">$C$38</f>
+        <v>Abdalla</v>
       </c>
       <c r="H98" s="0" t="str">
-        <f aca="false">$C$81</f>
-        <v>Fadwa</v>
+        <f aca="false">$C$39</f>
+        <v>Hikmat</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,152 +2801,127 @@
         <f aca="false">ROW()</f>
         <v>99</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C99" s="0" t="s">
+      <c r="B99" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D99" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E99" s="4" t="n">
-        <v>18537</v>
-      </c>
-      <c r="G99" s="0" t="str">
+      <c r="D99" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>100</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G100" s="0" t="str">
+        <f aca="false">$C$99</f>
+        <v>Asad</v>
+      </c>
+      <c r="H100" s="0" t="str">
+        <f aca="false">$C$98</f>
+        <v>Farihan</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>101</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>102</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G102" s="0" t="str">
+        <f aca="false">$C$101</f>
+        <v>Bryan</v>
+      </c>
+      <c r="H102" s="0" t="str">
+        <f aca="false">$C$100</f>
+        <v>Zana</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>103</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G103" s="0" t="str">
+        <f aca="false">$C$99</f>
+        <v>Asad</v>
+      </c>
+      <c r="H103" s="0" t="str">
+        <f aca="false">$C$98</f>
+        <v>Farihan</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>104</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G104" s="0" t="str">
         <f aca="false">$C$38</f>
         <v>Abdalla</v>
       </c>
-      <c r="H99" s="0" t="str">
+      <c r="H104" s="0" t="str">
         <f aca="false">$C$39</f>
         <v>Hikmat</v>
       </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="n">
-        <f aca="false">ROW()</f>
-        <v>100</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="n">
-        <f aca="false">ROW()</f>
-        <v>101</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C101" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G101" s="0" t="str">
-        <f aca="false">$C$100</f>
-        <v>Asad</v>
-      </c>
-      <c r="H101" s="0" t="str">
-        <f aca="false">$C$99</f>
-        <v>Farihan</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="n">
-        <f aca="false">ROW()</f>
-        <v>102</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="n">
-        <f aca="false">ROW()</f>
-        <v>103</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C103" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G103" s="0" t="str">
-        <f aca="false">$C$102</f>
-        <v>Bryan</v>
-      </c>
-      <c r="H103" s="0" t="str">
-        <f aca="false">$C$101</f>
-        <v>Zana</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="n">
-        <f aca="false">ROW()</f>
-        <v>104</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C104" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G104" s="0" t="str">
-        <f aca="false">$C$100</f>
-        <v>Asad</v>
-      </c>
-      <c r="H104" s="0" t="str">
-        <f aca="false">$C$99</f>
-        <v>Farihan</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="n">
-        <f aca="false">ROW()</f>
-        <v>105</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C105" s="0" t="s">
+      <c r="I104" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="D105" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G105" s="0" t="str">
-        <f aca="false">$C$38</f>
-        <v>Abdalla</v>
-      </c>
-      <c r="H105" s="0" t="str">
-        <f aca="false">$C$39</f>
-        <v>Hikmat</v>
-      </c>
-      <c r="I105" s="0" t="s">
-        <v>128</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added Aisha and Wasfiyya part of the family
</commit_message>
<xml_diff>
--- a/bushnaq.xlsx
+++ b/bushnaq.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="155">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -404,6 +404,87 @@
   </si>
   <si>
     <t xml:space="preserve">Born ~1953, died 1966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aisha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohammad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muhammad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dima?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riyad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mirna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ziyad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hanija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nasser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anwar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wasfiyya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadiq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zaina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadeq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Randa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dalal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rima</t>
   </si>
 </sst>
 </file>
@@ -634,13 +715,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G83" activeCellId="0" sqref="G83"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C150" activeCellId="0" sqref="C150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -2921,7 +3002,838 @@
         <v>127</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>105</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G105" s="0" t="str">
+        <f aca="false">C$2</f>
+        <v>Mustafa</v>
+      </c>
+      <c r="H105" s="0" t="str">
+        <f aca="false">$C$3</f>
+        <v>Bahiyya</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>106</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>107</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="G107" s="0" t="str">
+        <f aca="false">$C$106</f>
+        <v>Mohammad</v>
+      </c>
+      <c r="H107" s="0" t="str">
+        <f aca="false">$C$105</f>
+        <v>Aisha</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>108</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>109</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="G109" s="0" t="str">
+        <f aca="false">$C$107</f>
+        <v>Akram</v>
+      </c>
+      <c r="H109" s="0" t="str">
+        <f aca="false">$C$108</f>
+        <v>??</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>110</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="G110" s="0" t="str">
+        <f aca="false">$C$107</f>
+        <v>Akram</v>
+      </c>
+      <c r="H110" s="0" t="str">
+        <f aca="false">$C$108</f>
+        <v>??</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>111</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G111" s="0" t="str">
+        <f aca="false">$C$107</f>
+        <v>Akram</v>
+      </c>
+      <c r="H111" s="0" t="str">
+        <f aca="false">$C$108</f>
+        <v>??</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>112</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="G112" s="0" t="str">
+        <f aca="false">$C$106</f>
+        <v>Mohammad</v>
+      </c>
+      <c r="H112" s="0" t="str">
+        <f aca="false">$C$105</f>
+        <v>Aisha</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>113</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>114</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="G114" s="0" t="str">
+        <f aca="false">$C$112</f>
+        <v>Riyad</v>
+      </c>
+      <c r="H114" s="0" t="str">
+        <f aca="false">$C$113</f>
+        <v>??</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>115</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>116</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G116" s="0" t="str">
+        <f aca="false">$C$115</f>
+        <v>??</v>
+      </c>
+      <c r="H116" s="0" t="str">
+        <f aca="false">$C$114</f>
+        <v>Mirna</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>117</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G117" s="0" t="str">
+        <f aca="false">$C$115</f>
+        <v>??</v>
+      </c>
+      <c r="H117" s="0" t="str">
+        <f aca="false">$C$114</f>
+        <v>Mirna</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>118</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="G118" s="0" t="str">
+        <f aca="false">$C$112</f>
+        <v>Riyad</v>
+      </c>
+      <c r="H118" s="0" t="str">
+        <f aca="false">$C$113</f>
+        <v>??</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>119</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>120</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G120" s="0" t="str">
+        <f aca="false">$C$119</f>
+        <v>??</v>
+      </c>
+      <c r="H120" s="0" t="str">
+        <f aca="false">$C$118</f>
+        <v>Rajai</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>121</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="G121" s="0" t="str">
+        <f aca="false">$C$112</f>
+        <v>Riyad</v>
+      </c>
+      <c r="H121" s="0" t="str">
+        <f aca="false">$C$113</f>
+        <v>??</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>122</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G122" s="0" t="str">
+        <f aca="false">$C$106</f>
+        <v>Mohammad</v>
+      </c>
+      <c r="H122" s="0" t="str">
+        <f aca="false">$C$105</f>
+        <v>Aisha</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>123</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>124</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G124" s="0" t="str">
+        <f aca="false">$C$122</f>
+        <v>Ziyad</v>
+      </c>
+      <c r="H124" s="0" t="str">
+        <f aca="false">$C$123</f>
+        <v>??</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>125</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G125" s="0" t="str">
+        <f aca="false">$C$122</f>
+        <v>Ziyad</v>
+      </c>
+      <c r="H125" s="0" t="str">
+        <f aca="false">$C$123</f>
+        <v>??</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>126</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="G126" s="0" t="str">
+        <f aca="false">$C$122</f>
+        <v>Ziyad</v>
+      </c>
+      <c r="H126" s="0" t="str">
+        <f aca="false">$C$123</f>
+        <v>??</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>127</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G127" s="0" t="str">
+        <f aca="false">$C$106</f>
+        <v>Mohammad</v>
+      </c>
+      <c r="H127" s="0" t="str">
+        <f aca="false">$C$105</f>
+        <v>Aisha</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>128</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>129</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="G129" s="0" t="str">
+        <f aca="false">$C$127</f>
+        <v>Ali</v>
+      </c>
+      <c r="H129" s="0" t="str">
+        <f aca="false">$C$128</f>
+        <v>Hanija</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>130</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G130" s="0" t="str">
+        <f aca="false">$C$127</f>
+        <v>Ali</v>
+      </c>
+      <c r="H130" s="0" t="str">
+        <f aca="false">$C$128</f>
+        <v>Hanija</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>131</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="G131" s="0" t="str">
+        <f aca="false">$C$106</f>
+        <v>Mohammad</v>
+      </c>
+      <c r="H131" s="0" t="str">
+        <f aca="false">$C$105</f>
+        <v>Aisha</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>132</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>133</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="G133" s="0" t="str">
+        <f aca="false">$C$132</f>
+        <v>Sadiq</v>
+      </c>
+      <c r="H133" s="0" t="str">
+        <f aca="false">$C$131</f>
+        <v>Wasfiyya</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>134</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>135</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G135" s="0" t="str">
+        <f aca="false">$C$134</f>
+        <v>??</v>
+      </c>
+      <c r="H135" s="0" t="str">
+        <f aca="false">$C$133</f>
+        <v>Maha</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>136</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C136" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="G136" s="0" t="str">
+        <f aca="false">$C$134</f>
+        <v>??</v>
+      </c>
+      <c r="H136" s="0" t="str">
+        <f aca="false">$C$133</f>
+        <v>Maha</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>137</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="G137" s="0" t="str">
+        <f aca="false">$C$134</f>
+        <v>??</v>
+      </c>
+      <c r="H137" s="0" t="str">
+        <f aca="false">$C$133</f>
+        <v>Maha</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>138</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C138" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G138" s="0" t="str">
+        <f aca="false">$C$134</f>
+        <v>??</v>
+      </c>
+      <c r="H138" s="0" t="str">
+        <f aca="false">$C$133</f>
+        <v>Maha</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>139</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C139" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G139" s="0" t="str">
+        <f aca="false">$C$132</f>
+        <v>Sadiq</v>
+      </c>
+      <c r="H139" s="0" t="str">
+        <f aca="false">$C$131</f>
+        <v>Wasfiyya</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>140</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G140" s="0" t="str">
+        <f aca="false">$C$132</f>
+        <v>Sadiq</v>
+      </c>
+      <c r="H140" s="0" t="str">
+        <f aca="false">$C$131</f>
+        <v>Wasfiyya</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>141</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C141" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>142</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C142" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="G142" s="0" t="str">
+        <f aca="false">$C$140</f>
+        <v>Maher</v>
+      </c>
+      <c r="H142" s="0" t="str">
+        <f aca="false">$C$141</f>
+        <v>??</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>143</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G143" s="0" t="str">
+        <f aca="false">$C$140</f>
+        <v>Maher</v>
+      </c>
+      <c r="H143" s="0" t="str">
+        <f aca="false">$C$141</f>
+        <v>??</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>144</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C144" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="G144" s="0" t="str">
+        <f aca="false">$C$132</f>
+        <v>Sadiq</v>
+      </c>
+      <c r="H144" s="0" t="str">
+        <f aca="false">$C$131</f>
+        <v>Wasfiyya</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>145</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="G145" s="0" t="str">
+        <f aca="false">$C$132</f>
+        <v>Sadiq</v>
+      </c>
+      <c r="H145" s="0" t="str">
+        <f aca="false">$C$131</f>
+        <v>Wasfiyya</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>146</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>147</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G147" s="0" t="str">
+        <f aca="false">$C$146</f>
+        <v>??</v>
+      </c>
+      <c r="H147" s="0" t="str">
+        <f aca="false">$C$145</f>
+        <v>Dalal</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>148</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C148" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G148" s="0" t="str">
+        <f aca="false">$C$146</f>
+        <v>??</v>
+      </c>
+      <c r="H148" s="0" t="str">
+        <f aca="false">$C$145</f>
+        <v>Dalal</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>149</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C149" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G149" s="0" t="str">
+        <f aca="false">$C$146</f>
+        <v>??</v>
+      </c>
+      <c r="H149" s="0" t="str">
+        <f aca="false">$C$145</f>
+        <v>Dalal</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="n">
+        <f aca="false">ROW()</f>
+        <v>150</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C150" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="G150" s="0" t="str">
+        <f aca="false">$C$132</f>
+        <v>Sadiq</v>
+      </c>
+      <c r="H150" s="0" t="str">
+        <f aca="false">$C$131</f>
+        <v>Wasfiyya</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>